<commit_message>
Added minor courses and fixed icons
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_DSAI_post_mid_timetable.xlsx
+++ b/backend/output_timetables/sem1_DSAI_post_mid_timetable.xlsx
@@ -1087,16 +1087,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>6.25</v>
+        <v>0</v>
       </c>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -1355,16 +1355,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [C001]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2526,7 +2526,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [C001]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3450,7 +3450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M114"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3964,15 +3964,19 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Hardware Lab</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Equipment</t>
+        </is>
+      </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
@@ -3984,7 +3988,7 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>L105</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -4019,15 +4023,19 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Hardware Lab</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr"/>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Equipment</t>
+        </is>
+      </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
@@ -4039,7 +4047,7 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>L105</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -4364,7 +4372,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -4427,7 +4435,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -4490,7 +4498,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -4553,7 +4561,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -4616,7 +4624,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -4679,7 +4687,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -4742,7 +4750,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -4805,7 +4813,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -4868,7 +4876,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -4931,7 +4939,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -4994,7 +5002,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -5057,7 +5065,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13:00-14:30</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -5070,11 +5078,7 @@
           <t>120</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="b">
         <v>0</v>
       </c>
@@ -5086,12 +5090,12 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C001</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>DS161</t>
         </is>
       </c>
     </row>
@@ -5111,22 +5115,22 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15:30-17:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -5145,12 +5149,12 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>MA162</t>
         </is>
       </c>
     </row>
@@ -5170,27 +5174,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>240</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>Audio/Video System</t>
         </is>
       </c>
       <c r="I29" t="b">
@@ -5201,15 +5205,19 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>PH151</t>
         </is>
       </c>
     </row>
@@ -5229,12 +5237,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -5260,7 +5268,11 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L30" t="inlineStr">
         <is>
           <t>C004</t>
@@ -5268,7 +5280,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>DS151</t>
         </is>
       </c>
     </row>
@@ -5288,12 +5300,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -5319,7 +5331,11 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L31" t="inlineStr">
         <is>
           <t>C004</t>
@@ -5327,7 +5343,7 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -5347,12 +5363,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -5378,7 +5394,11 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L32" t="inlineStr">
         <is>
           <t>C004</t>
@@ -5386,7 +5406,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>CS151</t>
         </is>
       </c>
     </row>
@@ -5406,27 +5426,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>240</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>Audio/Video System</t>
         </is>
       </c>
       <c r="I33" t="b">
@@ -5437,15 +5457,19 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>HS157</t>
         </is>
       </c>
     </row>
@@ -5470,7 +5494,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -5508,7 +5532,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>HS102</t>
         </is>
       </c>
     </row>
@@ -5533,7 +5557,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -5571,7 +5595,7 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>DS151</t>
+          <t>HS103</t>
         </is>
       </c>
     </row>
@@ -5596,7 +5620,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -5634,7 +5658,7 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>DE101</t>
         </is>
       </c>
     </row>
@@ -5659,7 +5683,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -5697,7 +5721,7 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>HS156</t>
         </is>
       </c>
     </row>
@@ -5722,7 +5746,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -5760,7 +5784,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>HS152</t>
         </is>
       </c>
     </row>
@@ -5785,7 +5809,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -5823,7 +5847,7 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>HS102</t>
+          <t>CS161</t>
         </is>
       </c>
     </row>
@@ -5848,22 +5872,22 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>Hardware Lab</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>40</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Equipment</t>
         </is>
       </c>
       <c r="I40" t="b">
@@ -5874,19 +5898,15 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
+      <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>L105</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>HS103</t>
+          <t>EC161 (Lab)</t>
         </is>
       </c>
     </row>
@@ -5906,12 +5926,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>13:00-14:30</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5930,18 +5950,14 @@
         </is>
       </c>
       <c r="I41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
+      <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
           <t>C004</t>
@@ -5949,7 +5965,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>DE101</t>
+          <t>EC161 (Lab)</t>
         </is>
       </c>
     </row>
@@ -5969,27 +5985,27 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>Hardware Lab</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>40</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Equipment</t>
         </is>
       </c>
       <c r="I42" t="b">
@@ -6000,19 +6016,15 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
+      <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>L206</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>EC161 (Lab)</t>
         </is>
       </c>
     </row>
@@ -6032,12 +6044,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -6075,7 +6087,7 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>HS152</t>
+          <t>HS157</t>
         </is>
       </c>
     </row>
@@ -6095,12 +6107,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -6138,7 +6150,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>HS156</t>
         </is>
       </c>
     </row>
@@ -6158,12 +6170,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -6189,7 +6201,11 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L45" t="inlineStr">
         <is>
           <t>C004</t>
@@ -6197,7 +6213,7 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>HS152</t>
         </is>
       </c>
     </row>
@@ -6217,27 +6233,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>240</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>Audio/Video System</t>
         </is>
       </c>
       <c r="I46" t="b">
@@ -6248,15 +6264,19 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
+          <t>PH151</t>
         </is>
       </c>
     </row>
@@ -6276,12 +6296,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -6307,7 +6327,11 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L47" t="inlineStr">
         <is>
           <t>C004</t>
@@ -6315,7 +6339,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
+          <t>DS151</t>
         </is>
       </c>
     </row>
@@ -6335,12 +6359,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -6378,7 +6402,7 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -6398,12 +6422,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -6441,7 +6465,7 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>HS102</t>
         </is>
       </c>
     </row>
@@ -6461,12 +6485,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6504,7 +6528,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>HS152</t>
+          <t>HS103</t>
         </is>
       </c>
     </row>
@@ -6524,12 +6548,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6567,7 +6591,7 @@
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>DE101</t>
         </is>
       </c>
     </row>
@@ -6587,12 +6611,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6630,7 +6654,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>DS151</t>
+          <t>CS151</t>
         </is>
       </c>
     </row>
@@ -6650,12 +6674,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6693,3802 +6717,7 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>CS101</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>1</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I54" t="b">
-        <v>0</v>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>HS102</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>1</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I55" t="b">
-        <v>0</v>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>HS103</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>1</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I56" t="b">
-        <v>0</v>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>DE101</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>1</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I57" t="b">
-        <v>0</v>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>CS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>1</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I58" t="b">
-        <v>0</v>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
-        <is>
           <t>CS161</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>1</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I59" t="b">
-        <v>0</v>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>HS157</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>1</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I60" t="b">
-        <v>0</v>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>HS156</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I61" t="b">
-        <v>0</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>HS152</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>1</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I62" t="b">
-        <v>0</v>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>PH151</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>1</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I63" t="b">
-        <v>0</v>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>DS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>1</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I64" t="b">
-        <v>0</v>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>CS101</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>1</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I65" t="b">
-        <v>0</v>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>HS102</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>1</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I66" t="b">
-        <v>0</v>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>HS103</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>1</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I67" t="b">
-        <v>0</v>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>DE101</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>1</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I68" t="b">
-        <v>0</v>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>CS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>1</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>09:00-10:30</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I69" t="b">
-        <v>0</v>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>1</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Thu</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>13:00-14:30</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I70" t="b">
-        <v>0</v>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr"/>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>EC161 (Lab)</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>1</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Thu</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>Hardware Lab</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>Equipment</t>
-        </is>
-      </c>
-      <c r="I71" t="b">
-        <v>0</v>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr"/>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>L206</t>
-        </is>
-      </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>EC161 (Lab)</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>1</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I72" t="b">
-        <v>0</v>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>HS157</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>1</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I73" t="b">
-        <v>0</v>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>HS156</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>1</v>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I74" t="b">
-        <v>0</v>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>HS152</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>1</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I75" t="b">
-        <v>0</v>
-      </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>PH151</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>1</v>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I76" t="b">
-        <v>0</v>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>DS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>1</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I77" t="b">
-        <v>0</v>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>CS101</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>1</v>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I78" t="b">
-        <v>0</v>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>HS102</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>1</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I79" t="b">
-        <v>0</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>HS103</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>1</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I80" t="b">
-        <v>0</v>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>DE101</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>1</v>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I81" t="b">
-        <v>0</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>CS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>1</v>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I82" t="b">
-        <v>0</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>1</v>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I83" t="b">
-        <v>0</v>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>PH151</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>1</v>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I84" t="b">
-        <v>0</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>DS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>1</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I85" t="b">
-        <v>0</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>CS101</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>1</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I86" t="b">
-        <v>0</v>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>CS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>1</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I87" t="b">
-        <v>0</v>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>HS157</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>1</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I88" t="b">
-        <v>0</v>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>HS102</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>1</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I89" t="b">
-        <v>0</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>HS103</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>1</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I90" t="b">
-        <v>0</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>DE101</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>1</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I91" t="b">
-        <v>0</v>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>HS156</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>1</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I92" t="b">
-        <v>0</v>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>HS152</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>1</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I93" t="b">
-        <v>0</v>
-      </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>1</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>large classroom</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I94" t="b">
-        <v>0</v>
-      </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>MA161</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>1</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>large classroom</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I95" t="b">
-        <v>0</v>
-      </c>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>DS161</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>1</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>large classroom</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I96" t="b">
-        <v>0</v>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr"/>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>1</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I97" t="b">
-        <v>0</v>
-      </c>
-      <c r="J97" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>MA161</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>1</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I98" t="b">
-        <v>0</v>
-      </c>
-      <c r="J98" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>DS161</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>1</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I99" t="b">
-        <v>0</v>
-      </c>
-      <c r="J99" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K99" t="inlineStr"/>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>1</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>large classroom</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I100" t="b">
-        <v>0</v>
-      </c>
-      <c r="J100" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K100" t="inlineStr"/>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>1</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I101" t="b">
-        <v>0</v>
-      </c>
-      <c r="J101" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>PH151</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>1</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I102" t="b">
-        <v>0</v>
-      </c>
-      <c r="J102" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L102" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>DS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>1</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I103" t="b">
-        <v>0</v>
-      </c>
-      <c r="J103" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L103" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>CS101</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>1</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I104" t="b">
-        <v>0</v>
-      </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>CS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>1</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I105" t="b">
-        <v>0</v>
-      </c>
-      <c r="J105" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L105" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M105" t="inlineStr">
-        <is>
-          <t>HS157</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>1</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I106" t="b">
-        <v>0</v>
-      </c>
-      <c r="J106" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K106" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L106" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M106" t="inlineStr">
-        <is>
-          <t>HS102</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>1</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I107" t="b">
-        <v>0</v>
-      </c>
-      <c r="J107" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L107" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M107" t="inlineStr">
-        <is>
-          <t>HS103</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>1</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I108" t="b">
-        <v>0</v>
-      </c>
-      <c r="J108" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K108" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L108" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M108" t="inlineStr">
-        <is>
-          <t>DE101</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>1</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I109" t="b">
-        <v>0</v>
-      </c>
-      <c r="J109" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L109" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>HS156</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>1</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I110" t="b">
-        <v>0</v>
-      </c>
-      <c r="J110" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K110" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L110" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>HS152</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>1</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I111" t="b">
-        <v>0</v>
-      </c>
-      <c r="J111" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L111" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M111" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>1</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I112" t="b">
-        <v>0</v>
-      </c>
-      <c r="J112" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K112" t="inlineStr"/>
-      <c r="L112" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>1</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>large classroom</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
-      <c r="I113" t="b">
-        <v>0</v>
-      </c>
-      <c r="J113" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K113" t="inlineStr"/>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
-      </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>EC161 (Lab)</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>1</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H114" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I114" t="b">
-        <v>0</v>
-      </c>
-      <c r="J114" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K114" t="inlineStr"/>
-      <c r="L114" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M114" t="inlineStr">
-        <is>
-          <t>EC161 (Lab)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added classroom allocation for invidual courses of elective baskets
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_DSAI_post_mid_timetable.xlsx
+++ b/backend/output_timetables/sem1_DSAI_post_mid_timetable.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,27 +481,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>07:30-09:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CS161 [C004]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MA161 [C303]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -513,27 +513,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10:30-12:00</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CS161 [C004]</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MA162 [C305]</t>
+          <t>CS161 [C101]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>EC161 [C101]</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>DS161 [C101]</t>
+          <t>MA161 [C002]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -545,118 +545,118 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>12:00-13:00</t>
+          <t>10:30-12:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>CS161 [C101]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>DS161 [C001]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>13:00-14:30</t>
+          <t>12:00-13:00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CS161 (Lab)</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MA161 [C004]</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>14:30-15:30</t>
+          <t>13:00-14:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [C004]</t>
+          <t>CS161 (Lab) [L403]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>EC161 [C004]</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>MA161 [C002]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Free</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1 (Tutorial)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>15:30-17:00</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>CS161 (Lab) [L403]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DS161 [C004]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -666,37 +666,101 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>ELECTIVE_B1 (Tutorial)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>15:30-17:00</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MA162 [C004]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>EC161 (Lab) [L105]</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>DS161 [C002]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>EC161 (Lab) [C001]</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>EC161 (Lab) [L105]</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>18:30-20:00</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
@@ -791,11 +855,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>HS157, HS156, HS152, CS151</t>
+          <t>HS152, HS157, HS156</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -824,7 +888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -877,7 +941,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>HS152</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -891,7 +955,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -912,7 +976,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -926,7 +990,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -947,7 +1011,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HS152</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -961,7 +1025,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -969,41 +1033,6 @@
         </is>
       </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>CS151</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Fri 14:30-15:30</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1087,16 +1116,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -1117,16 +1146,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>11.25</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1185,16 +1214,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>11.5</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
-        <v>2.3</v>
+        <v>1.2</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>28.75</v>
+        <v>15</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1831,16 +1860,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>3.75</v>
+        <v>0</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1899,16 +1928,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>3.75</v>
+        <v>0</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -2185,16 +2214,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -2281,7 +2310,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2324,27 +2353,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>07:30-09:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CS161 [C004]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MA161 [C303]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2356,27 +2385,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10:30-12:00</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CS161 [C004]</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MA162 [C305]</t>
+          <t>CS161 [C101]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>EC161 [C101]</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>DS161 [C101]</t>
+          <t>MA161 [C002]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2388,118 +2417,118 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>12:00-13:00</t>
+          <t>10:30-12:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>CS161 [C101]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>DS161 [C001]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>LUNCH BREAK</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>13:00-14:30</t>
+          <t>12:00-13:00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [C004]</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MA161 [C004]</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>LUNCH BREAK</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>14:30-15:30</t>
+          <t>13:00-14:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [C004]</t>
+          <t>CS161 (Lab) [L406]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>EC161 [C004]</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>MA161 [C002]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Free</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1 (Tutorial)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>15:30-17:00</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>CS161 (Lab) [L406]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DS161 [C004]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2509,37 +2538,101 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>ELECTIVE_B1 (Tutorial)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>15:30-17:00</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MA162 [C004]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>EC161 (Lab) [L105]</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>DS161 [C002]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>18:30-20:00</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
@@ -2589,12 +2682,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>HS152</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C205</t>
         </is>
       </c>
     </row>
@@ -2606,12 +2699,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C302</t>
         </is>
       </c>
     </row>
@@ -2623,12 +2716,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HS152</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C204</t>
         </is>
       </c>
     </row>
@@ -2640,12 +2733,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>PH151</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C101</t>
         </is>
       </c>
     </row>
@@ -2657,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>DS151</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C203</t>
         </is>
       </c>
     </row>
@@ -2674,7 +2767,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DS151</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2691,12 +2784,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>CS151</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C003</t>
         </is>
       </c>
     </row>
@@ -2713,7 +2806,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C202</t>
         </is>
       </c>
     </row>
@@ -2730,7 +2823,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C002</t>
         </is>
       </c>
     </row>
@@ -2747,7 +2840,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C102</t>
         </is>
       </c>
     </row>
@@ -2764,7 +2857,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C101, C104</t>
         </is>
       </c>
     </row>
@@ -2924,7 +3017,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>L403, C101</t>
         </is>
       </c>
     </row>
@@ -2971,7 +3064,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>C305, C004</t>
+          <t>C004</t>
         </is>
       </c>
     </row>
@@ -3018,7 +3111,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>C101, C001, C004</t>
+          <t>L105, C004</t>
         </is>
       </c>
     </row>
@@ -3065,7 +3158,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>C303, C004</t>
+          <t>C002</t>
         </is>
       </c>
     </row>
@@ -3112,7 +3205,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>C101, C004</t>
+          <t>C002, C001</t>
         </is>
       </c>
     </row>
@@ -3174,7 +3267,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3258,7 +3351,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
+          <t>DS161</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -3270,26 +3363,26 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>120</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -3297,42 +3390,42 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>EC161, CS161, MA161...</t>
+          <t>DS161, MA161</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>0.6</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C101</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>240</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>Audio/Video System</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -3344,19 +3437,19 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>DS161, EC161</t>
+          <t>MA162, EC161</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.4</t>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3371,11 +3464,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -3387,55 +3480,98 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>L105</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Hardware Lab</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Equipment</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>EC161 (Lab)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>L403</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>classroom</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>TV</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>CS161 (Lab)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.4</t>
         </is>
       </c>
     </row>
@@ -3450,7 +3586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3524,6 +3660,11 @@
           <t>course</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>session_type</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -3551,17 +3692,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I2" t="b">
@@ -3575,12 +3716,17 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>CS161</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -3610,17 +3756,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I3" t="b">
@@ -3634,12 +3780,17 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>L406</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>CS161 (Lab)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Lab</t>
         </is>
       </c>
     </row>
@@ -3669,17 +3820,17 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I4" t="b">
@@ -3693,12 +3844,17 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>L406</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
           <t>CS161 (Lab)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Lab</t>
         </is>
       </c>
     </row>
@@ -3760,6 +3916,11 @@
           <t>MA162</t>
         </is>
       </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Lecture</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -3787,17 +3948,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I6" t="b">
@@ -3811,12 +3972,17 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>CS161</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -3846,17 +4012,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>240</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Audio/Video System</t>
         </is>
       </c>
       <c r="I7" t="b">
@@ -3870,12 +4036,17 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
           <t>MA162</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -3937,6 +4108,11 @@
           <t>EC161</t>
         </is>
       </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Lecture</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -3996,6 +4172,11 @@
           <t>EC161 (Lab)</t>
         </is>
       </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Lab</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -4055,6 +4236,11 @@
           <t>EC161 (Lab)</t>
         </is>
       </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Lab</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -4082,17 +4268,17 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>240</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>Audio/Video System</t>
         </is>
       </c>
       <c r="I11" t="b">
@@ -4106,12 +4292,17 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>C101</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
           <t>EC161</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4141,17 +4332,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I12" t="b">
@@ -4165,12 +4356,17 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
           <t>MA161</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4200,17 +4396,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I13" t="b">
@@ -4224,12 +4420,17 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
           <t>DS161</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4259,17 +4460,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I14" t="b">
@@ -4283,12 +4484,17 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
           <t>MA161</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4318,19 +4524,15 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="b">
         <v>0</v>
       </c>
@@ -4342,12 +4544,17 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>C101</t>
+          <t>C001</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
           <t>DS161</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4377,17 +4584,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I16" t="b">
@@ -4405,12 +4612,17 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
           <t>PH151</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4440,17 +4652,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I17" t="b">
@@ -4468,12 +4680,17 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
           <t>DS151</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4539,6 +4756,11 @@
           <t>CS101</t>
         </is>
       </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Lecture</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -4566,17 +4788,17 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>135</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I19" t="b">
@@ -4594,12 +4816,17 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
           <t>CS151</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4629,17 +4856,17 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I20" t="b">
@@ -4657,12 +4884,17 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
           <t>HS157</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4692,17 +4924,17 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I21" t="b">
@@ -4720,12 +4952,17 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
           <t>HS102</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4755,17 +4992,17 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I22" t="b">
@@ -4783,12 +5020,17 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
           <t>HS103</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4818,17 +5060,17 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I23" t="b">
@@ -4846,12 +5088,17 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
           <t>DE101</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4881,17 +5128,17 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I24" t="b">
@@ -4909,12 +5156,17 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
           <t>HS156</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -4944,17 +5196,17 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I25" t="b">
@@ -4972,12 +5224,17 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
           <t>HS152</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5007,17 +5264,17 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I26" t="b">
@@ -5035,12 +5292,17 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
           <t>CS161</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5098,6 +5360,7 @@
           <t>DS161</t>
         </is>
       </c>
+      <c r="N27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -5115,12 +5378,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>15:30-17:00</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -5146,15 +5409,24 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>C302</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5184,17 +5456,17 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I29" t="b">
@@ -5212,12 +5484,17 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5280,7 +5557,12 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>DS151</t>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5310,17 +5592,17 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>135</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I31" t="b">
@@ -5338,12 +5620,17 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5373,17 +5660,17 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I32" t="b">
@@ -5401,12 +5688,17 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5436,17 +5728,17 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I33" t="b">
@@ -5464,12 +5756,17 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5499,17 +5796,17 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I34" t="b">
@@ -5527,12 +5824,17 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>HS102</t>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5562,17 +5864,17 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I35" t="b">
@@ -5590,12 +5892,17 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>HS103</t>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5625,17 +5932,17 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I36" t="b">
@@ -5653,12 +5960,17 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>DE101</t>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5688,17 +6000,17 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I37" t="b">
@@ -5716,12 +6028,17 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>HS152</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5751,17 +6068,17 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I38" t="b">
@@ -5779,12 +6096,17 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>HS152</t>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>Lecture</t>
         </is>
       </c>
     </row>
@@ -5809,22 +6131,22 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>Hardware Lab</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>40</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Equipment</t>
         </is>
       </c>
       <c r="I39" t="b">
@@ -5835,21 +6157,18 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
+      <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>L105</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>CS161</t>
-        </is>
-      </c>
+          <t>EC161 (Lab)</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -5867,7 +6186,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -5877,17 +6196,17 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Hardware Lab</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Equipment</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I40" t="b">
@@ -5898,15 +6217,24 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>L105</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -5926,46 +6254,55 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>13:00-14:30</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -5985,7 +6322,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -5995,17 +6332,17 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Hardware Lab</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>240</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Equipment</t>
+          <t>Audio/Video System</t>
         </is>
       </c>
       <c r="I42" t="b">
@@ -6016,15 +6353,24 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>L206</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -6054,17 +6400,17 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>135</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I43" t="b">
@@ -6082,12 +6428,17 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -6117,17 +6468,17 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I44" t="b">
@@ -6145,12 +6496,17 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -6180,17 +6536,17 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I45" t="b">
@@ -6208,12 +6564,17 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>HS152</t>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -6243,17 +6604,17 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I46" t="b">
@@ -6271,12 +6632,17 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -6306,17 +6672,17 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I47" t="b">
@@ -6334,12 +6700,17 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>DS151</t>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -6369,17 +6740,17 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I48" t="b">
@@ -6397,12 +6768,17 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -6432,17 +6808,17 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="I49" t="b">
@@ -6460,12 +6836,17 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>HS102</t>
+          <t>HS152</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -6495,17 +6876,17 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="I50" t="b">
@@ -6523,12 +6904,17 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>HS103</t>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
         </is>
       </c>
     </row>
@@ -6548,7 +6934,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -6558,17 +6944,17 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>Hardware Lab</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>40</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Equipment</t>
         </is>
       </c>
       <c r="I51" t="b">
@@ -6579,147 +6965,18 @@
           <t>Global Tracking (from internal map)</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
+      <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>L105</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>DE101</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>1</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I52" t="b">
-        <v>0</v>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>CS151</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>1</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>14:30-15:30</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>Auditorium</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Audio/Video System</t>
-        </is>
-      </c>
-      <c r="I53" t="b">
-        <v>0</v>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>Global Tracking (from internal map)</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>ELECTIVE_B1</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
+          <t>EC161 (Lab)</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7213,7 +7470,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2026-01-18 11:33</t>
+          <t>2026-01-19 23:36</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -7277,12 +7534,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5/36</t>
+          <t>6/36</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Utilization: 13.9%</t>
+          <t>Utilization: 16.7%</t>
         </is>
       </c>
     </row>
@@ -7299,12 +7556,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>24.3%</t>
+          <t>18.9%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>A: 48.6%, B: 0.0%</t>
+          <t>A: 37.8%, B: 0.0%</t>
         </is>
       </c>
     </row>
@@ -7326,7 +7583,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Score: 31.3/100</t>
+          <t>Score: 29.7/100</t>
         </is>
       </c>
     </row>

</xml_diff>